<commit_message>
modified:   .DS_Store 	new file:   data/.DS_Store
</commit_message>
<xml_diff>
--- a/input-data_files/授信部位/國內授信/國內企業授信.xlsx
+++ b/input-data_files/授信部位/國內授信/國內企業授信.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10714"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zhouzihan/Desktop/climate-stress-test-tool/input-data_files/授信部位/國內授信/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C872AB0A-5BAA-5643-B64A-CB3A33A75853}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{123630B1-7578-ED43-B843-22337032B75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4700" yWindow="500" windowWidth="27300" windowHeight="17500" xr2:uid="{81580E2C-D25D-D444-815D-3A318D2674D2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="34">
   <si>
     <t>擔保品價值</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -161,6 +161,10 @@
   </si>
   <si>
     <t>範例3</t>
+  </si>
+  <si>
+    <t>範例</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -200,7 +204,7 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="BiauKaiTC"/>
-      <charset val="136"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -555,7 +559,7 @@
   <dimension ref="A1:P69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18"/>
@@ -836,6 +840,56 @@
       </c>
       <c r="O7" s="1">
         <v>120</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="A8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E8" s="1">
+        <v>20000</v>
+      </c>
+      <c r="F8" s="1">
+        <v>160</v>
+      </c>
+      <c r="G8" s="1">
+        <v>120</v>
+      </c>
+      <c r="H8" s="1">
+        <v>100000</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M8" s="1">
+        <v>200</v>
+      </c>
+      <c r="N8" s="1">
+        <v>75</v>
+      </c>
+      <c r="O8" s="1">
+        <v>120</v>
+      </c>
+      <c r="P8" s="1">
+        <v>100</v>
       </c>
     </row>
     <row r="16" spans="1:16">

</xml_diff>